<commit_message>
Subo algunas imágenes de simulaciones y mediciones al repo.
</commit_message>
<xml_diff>
--- a/mediciones/Q_Point/Q1.xlsx
+++ b/mediciones/Q_Point/Q1.xlsx
@@ -506,7 +506,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -766,11 +766,15 @@
         <f t="shared" si="0"/>
         <v>2.492188E-2</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
+      <c r="E11" s="9">
+        <v>2.95</v>
+      </c>
+      <c r="F11" s="9">
+        <v>9.4000000000000004E-3</v>
+      </c>
       <c r="G11" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.7730000000000001E-2</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
@@ -787,7 +791,9 @@
         <f t="shared" si="0"/>
         <v>9.9354380999999992E-2</v>
       </c>
-      <c r="E12" s="9"/>
+      <c r="E12" s="9">
+        <v>14.21</v>
+      </c>
       <c r="F12" s="9"/>
       <c r="G12" s="8">
         <f t="shared" si="1"/>
@@ -808,7 +814,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E13" s="9"/>
+      <c r="E13" s="9">
+        <v>19.82</v>
+      </c>
       <c r="F13" s="9"/>
       <c r="G13" s="8">
         <f t="shared" si="1"/>
@@ -829,7 +837,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E14" s="9"/>
+      <c r="E14" s="9">
+        <v>20.04</v>
+      </c>
       <c r="F14" s="9"/>
       <c r="G14" s="8">
         <f t="shared" si="1"/>
@@ -850,7 +860,9 @@
         <f t="shared" si="0"/>
         <v>0.11077136</v>
       </c>
-      <c r="E15" s="9"/>
+      <c r="E15" s="9">
+        <v>14.39</v>
+      </c>
       <c r="F15" s="9"/>
       <c r="G15" s="8">
         <f t="shared" si="1"/>
@@ -871,7 +883,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E16" s="9"/>
+      <c r="E16" s="9">
+        <v>20.03</v>
+      </c>
       <c r="F16" s="9"/>
       <c r="G16" s="8">
         <f t="shared" si="1"/>
@@ -892,7 +906,9 @@
         <f t="shared" si="0"/>
         <v>1.3626061399999998</v>
       </c>
-      <c r="E17" s="9"/>
+      <c r="E17" s="9">
+        <v>15</v>
+      </c>
       <c r="F17" s="9"/>
       <c r="G17" s="8">
         <f t="shared" si="1"/>
@@ -913,7 +929,9 @@
         <f t="shared" si="0"/>
         <v>1.3754114279999998</v>
       </c>
-      <c r="E18" s="9"/>
+      <c r="E18" s="9">
+        <v>14.85</v>
+      </c>
       <c r="F18" s="9"/>
       <c r="G18" s="8">
         <f t="shared" si="1"/>
@@ -934,7 +952,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E19" s="9"/>
+      <c r="E19" s="9">
+        <v>20.23</v>
+      </c>
       <c r="F19" s="9"/>
       <c r="G19" s="8">
         <f t="shared" si="1"/>
@@ -955,7 +975,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E20" s="9"/>
+      <c r="E20" s="9">
+        <v>1.27</v>
+      </c>
       <c r="F20" s="9"/>
       <c r="G20" s="8">
         <f t="shared" si="1"/>
@@ -976,7 +998,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E21" s="12"/>
+      <c r="E21" s="12">
+        <v>1.26</v>
+      </c>
       <c r="F21" s="12"/>
       <c r="G21" s="13">
         <f t="shared" si="1"/>
@@ -996,7 +1020,7 @@
       </c>
       <c r="G22" s="6">
         <f>SUM(G3:G21)</f>
-        <v>0.64359116894000001</v>
+        <v>0.67132116894000005</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">

</xml_diff>